<commit_message>
+added RTS sub fees
</commit_message>
<xml_diff>
--- a/Dropship/Origin.xlsx
+++ b/Dropship/Origin.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Documents\Work\Skyzer\Billing Template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\Finance\Billing Template\Upstream\Dropship\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{811C255D-EE6A-4660-BB1D-C2D468AC957E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC21ECD0-01F9-46C1-9C8C-C3EA681ED306}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="5145" windowWidth="29040" windowHeight="16440" activeTab="5" xr2:uid="{00A1F220-B496-4644-BB55-836357F490EA}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" activeTab="5" xr2:uid="{00A1F220-B496-4644-BB55-836357F490EA}"/>
   </bookViews>
   <sheets>
     <sheet name="Shipped SKU" sheetId="1" r:id="rId1"/>
@@ -20,18 +20,31 @@
     <sheet name="Type Summary" sheetId="6" r:id="rId5"/>
     <sheet name="Summary" sheetId="10" r:id="rId6"/>
     <sheet name="Errors" sheetId="9" r:id="rId7"/>
+    <sheet name="Materials" sheetId="11" r:id="rId8"/>
+    <sheet name="Types" sheetId="12" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="74">
   <si>
     <t>SKU</t>
   </si>
@@ -156,9 +169,6 @@
     <t>satchel_ctp3</t>
   </si>
   <si>
-    <t>RTS - Processing of RTS Returns, Unpack, Inspection, De-Trash, Scan, Sorting and Report</t>
-  </si>
-  <si>
     <t>Labour - Labour Rate Weekday</t>
   </si>
   <si>
@@ -205,6 +215,57 @@
   </si>
   <si>
     <t>Dropship Order Fulfillment - Single Item Order (NC)</t>
+  </si>
+  <si>
+    <t>Vendor</t>
+  </si>
+  <si>
+    <t>Material</t>
+  </si>
+  <si>
+    <t>Ordered</t>
+  </si>
+  <si>
+    <t>Fulfilled</t>
+  </si>
+  <si>
+    <t>origin_internet</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>4842</t>
+  </si>
+  <si>
+    <t>3919</t>
+  </si>
+  <si>
+    <t>854</t>
+  </si>
+  <si>
+    <t>82</t>
+  </si>
+  <si>
+    <t>69</t>
+  </si>
+  <si>
+    <t>Type Ref</t>
+  </si>
+  <si>
+    <t>Type Name</t>
+  </si>
+  <si>
+    <t>4829</t>
+  </si>
+  <si>
+    <t>Origin – Processing of RTS Returns – Pristine (Return to Stock)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Origin – Processing of RTS Returns – Refurbishment Pathway </t>
+  </si>
+  <si>
+    <t>Origin – Processing of RTS Returns – BER/Non-Refurbishment</t>
   </si>
 </sst>
 </file>
@@ -722,7 +783,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="4" xfId="10" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -778,6 +839,12 @@
     <xf numFmtId="0" fontId="16" fillId="20" borderId="0" xfId="30" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" xfId="10" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="20" builtinId="30" customBuiltin="1"/>
@@ -825,6 +892,15 @@
     <cellStyle name="Warning Text" xfId="15" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="30">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -992,15 +1068,6 @@
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
@@ -1088,10 +1155,10 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C3DE09D7-D422-4DAA-A816-08D2DF870459}" name="Rate" displayName="Rate" ref="A1:K7" totalsRowShown="0" dataCellStyle="Normal">
-  <autoFilter ref="A1:K7" xr:uid="{C3DE09D7-D422-4DAA-A816-08D2DF870459}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J15">
-    <sortCondition ref="A1:A15"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C3DE09D7-D422-4DAA-A816-08D2DF870459}" name="Rate" displayName="Rate" ref="A1:K9" totalsRowShown="0" dataCellStyle="Normal">
+  <autoFilter ref="A1:K9" xr:uid="{C3DE09D7-D422-4DAA-A816-08D2DF870459}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J14">
+    <sortCondition ref="A1:A14"/>
   </sortState>
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{24F70D57-2EE1-4C0C-AB27-FA9936CA2FDA}" name="SAP Code" dataCellStyle="Normal"/>
@@ -1100,7 +1167,7 @@
     <tableColumn id="7" xr3:uid="{B071484C-D0BA-4C96-9047-56AA6FAE2695}" name="Orders" dataCellStyle="Calculation">
       <calculatedColumnFormula>SUMIF(Type[Ship Code], Rate[[#This Row],[SAP Code]], Type[Ship Qty])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{B6314D7F-E2BD-4447-91E9-B45887035D99}" name="Boxes" dataDxfId="22" dataCellStyle="Calculation">
+    <tableColumn id="11" xr3:uid="{B6314D7F-E2BD-4447-91E9-B45887035D99}" name="Boxes" dataDxfId="2" dataCellStyle="Calculation">
       <calculatedColumnFormula>SUMIF(Type[Box Code], Rate[[#This Row],[SAP Code]], Type[Box Qty])</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="10" xr3:uid="{D36CB0F0-B99E-4655-8240-3D29B34D47F2}" name="Shipped" dataCellStyle="Calculation">
@@ -1112,13 +1179,13 @@
     <tableColumn id="9" xr3:uid="{A631A77F-4C93-47BA-B2F5-87087DAEEB42}" name="Commissioned" dataCellStyle="Calculation">
       <calculatedColumnFormula>SUMIF(SKU[Commission Code], Rate[[#This Row],[SAP Code]], SKU[Ship Qty])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{43ECE4A2-7997-4541-9CF5-E9D0E002B84A}" name="Qty" dataDxfId="21" dataCellStyle="Output">
+    <tableColumn id="6" xr3:uid="{43ECE4A2-7997-4541-9CF5-E9D0E002B84A}" name="Qty" dataDxfId="1" dataCellStyle="Output">
       <calculatedColumnFormula>SUM(Rate[[#This Row],[Orders]:[Commissioned]])</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="5" xr3:uid="{061815EC-389D-41AD-8624-476B7BDF7EF9}" name="Cost" dataCellStyle="Currency">
       <calculatedColumnFormula>Rate[[#This Row],[Rate]]*Rate[[#This Row],[Qty]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{3DA820DC-EBEF-4FE5-9A43-78816C2BB57F}" name="Error" dataDxfId="20" dataCellStyle="Normal">
+    <tableColumn id="4" xr3:uid="{3DA820DC-EBEF-4FE5-9A43-78816C2BB57F}" name="Error" dataDxfId="0" dataCellStyle="Normal">
       <calculatedColumnFormula>IF(ISNA(MATCH(Rate[[#This Row],[SAP Code]], Summary!A:A, 0)), _xlfn.CONCAT("Missing ", Rate[[#This Row],[SAP Code]], " in summary"), "")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1130,31 +1197,31 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{3408F06A-19C6-485A-BFD6-642AAEDC81AB}" name="SKU" displayName="SKU" ref="A1:M7" totalsRowShown="0">
   <autoFilter ref="A1:M7" xr:uid="{3408F06A-19C6-485A-BFD6-642AAEDC81AB}"/>
   <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{D34CFDBF-6E27-474A-96EE-C62F3857D517}" name="SKU" dataDxfId="19"/>
-    <tableColumn id="2" xr3:uid="{31BC9093-55B2-47F4-AC5E-20202B2E6550}" name="Name" dataDxfId="18"/>
-    <tableColumn id="3" xr3:uid="{531877B5-9C86-4C0D-9CBB-838D9F308DF1}" name="Ship Code" dataDxfId="17" dataCellStyle="Input"/>
-    <tableColumn id="4" xr3:uid="{7088BE2B-D88F-4C34-8161-100B57F8FB78}" name="Ship Qty" dataDxfId="16" dataCellStyle="Calculation">
+    <tableColumn id="1" xr3:uid="{D34CFDBF-6E27-474A-96EE-C62F3857D517}" name="SKU" dataDxfId="22"/>
+    <tableColumn id="2" xr3:uid="{31BC9093-55B2-47F4-AC5E-20202B2E6550}" name="Name" dataDxfId="21"/>
+    <tableColumn id="3" xr3:uid="{531877B5-9C86-4C0D-9CBB-838D9F308DF1}" name="Ship Code" dataDxfId="20" dataCellStyle="Input"/>
+    <tableColumn id="4" xr3:uid="{7088BE2B-D88F-4C34-8161-100B57F8FB78}" name="Ship Qty" dataDxfId="19" dataCellStyle="Calculation">
       <calculatedColumnFormula>SUMIF(Ship_SKU[SKU], SKU[[#This Row],[SKU]], Ship_SKU[Qty])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{B9C37E4C-73B3-4F6A-A718-1097B41D1E93}" name="Ship Cost" dataDxfId="15" dataCellStyle="Currency">
+    <tableColumn id="11" xr3:uid="{B9C37E4C-73B3-4F6A-A718-1097B41D1E93}" name="Ship Cost" dataDxfId="18" dataCellStyle="Currency">
       <calculatedColumnFormula>IF(SKU[[#This Row],[Ship Code]]="", 0, VLOOKUP(SKU[[#This Row],[Ship Code]], Rate[], 3, FALSE)*SKU[[#This Row],[Ship Qty]])</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="5" xr3:uid="{FB5DBA6D-00FD-4CED-8E0F-4F56D5A58EC5}" name="Kit Code" dataCellStyle="Input"/>
     <tableColumn id="6" xr3:uid="{687DD87B-20BA-46B9-B299-3A91BDAE14EC}" name="Kit Items" dataCellStyle="Normal"/>
-    <tableColumn id="14" xr3:uid="{4DBEE7C7-94EB-422A-9A5B-D62C4BDDD8E9}" name="Kit Qty" dataDxfId="14" dataCellStyle="Calculation">
+    <tableColumn id="14" xr3:uid="{4DBEE7C7-94EB-422A-9A5B-D62C4BDDD8E9}" name="Kit Qty" dataDxfId="17" dataCellStyle="Calculation">
       <calculatedColumnFormula>SKU[[#This Row],[Ship Qty]]*SKU[[#This Row],[Kit Items]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{5CCD393F-2453-4795-833A-23ECDF388B07}" name="Kit Cost" dataDxfId="13" dataCellStyle="Calculation">
+    <tableColumn id="12" xr3:uid="{5CCD393F-2453-4795-833A-23ECDF388B07}" name="Kit Cost" dataDxfId="16" dataCellStyle="Calculation">
       <calculatedColumnFormula>IF(SKU[[#This Row],[Kit Code]]="", 0, VLOOKUP(SKU[[#This Row],[Kit Code]], Rate[], 3, FALSE)*SKU[[#This Row],[Kit Qty]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{75ED25F9-159C-4388-8B09-7F5EE9FBF6F7}" name="Commission Code" dataDxfId="12" dataCellStyle="Input"/>
-    <tableColumn id="13" xr3:uid="{140E9353-875E-4671-AD80-72991CE58F6D}" name="Comission Cost" dataDxfId="11" dataCellStyle="Calculation">
+    <tableColumn id="7" xr3:uid="{75ED25F9-159C-4388-8B09-7F5EE9FBF6F7}" name="Commission Code" dataDxfId="15" dataCellStyle="Input"/>
+    <tableColumn id="13" xr3:uid="{140E9353-875E-4671-AD80-72991CE58F6D}" name="Comission Cost" dataDxfId="14" dataCellStyle="Calculation">
       <calculatedColumnFormula>IF(SKU[[#This Row],[Commission Code]]="", 0, VLOOKUP(SKU[[#This Row],[Commission Code]], Rate[], 3, FALSE)*SKU[[#This Row],[Ship Qty]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{6E734072-2A9B-43B4-A7B8-5682F9AC4C66}" name="Total" dataDxfId="10" dataCellStyle="Output">
+    <tableColumn id="8" xr3:uid="{6E734072-2A9B-43B4-A7B8-5682F9AC4C66}" name="Total" dataDxfId="13" dataCellStyle="Output">
       <calculatedColumnFormula>SKU[[#This Row],[Ship Cost]]+SKU[[#This Row],[Kit Cost]]+SKU[[#This Row],[Comission Cost]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{D23FACEE-5AD9-4665-B748-4AB1D0EFFD86}" name="Error" dataDxfId="9">
+    <tableColumn id="9" xr3:uid="{D23FACEE-5AD9-4665-B748-4AB1D0EFFD86}" name="Error" dataDxfId="12">
       <calculatedColumnFormula>IF(OR(ISNA(SKU[[#This Row],[Ship Cost]]), ISNA(SKU[[#This Row],[Kit Cost]]), ISNA(SKU[[#This Row],[Comission Cost]])), "Error Accessing SAP Rate", "")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1167,25 +1234,25 @@
   <autoFilter ref="A1:J2" xr:uid="{A3697F71-8505-4801-AFD3-DB4D2092ACE2}"/>
   <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{0B29E2D3-D0A7-41FB-85C2-6295CBE39907}" name="REF"/>
-    <tableColumn id="2" xr3:uid="{0D310FA7-648F-4BF4-8DC2-E720EFF9B487}" name="Name" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{A41ACBAE-7476-4350-B5AA-9FBA621C2301}" name="Ship Code" dataDxfId="7" dataCellStyle="Input"/>
-    <tableColumn id="4" xr3:uid="{0365826B-1DC9-4904-8CF1-A1C7B2EC0BA0}" name="Ship Qty" dataDxfId="6" dataCellStyle="Calculation">
+    <tableColumn id="2" xr3:uid="{0D310FA7-648F-4BF4-8DC2-E720EFF9B487}" name="Name" dataDxfId="11"/>
+    <tableColumn id="3" xr3:uid="{A41ACBAE-7476-4350-B5AA-9FBA621C2301}" name="Ship Code" dataDxfId="10" dataCellStyle="Input"/>
+    <tableColumn id="4" xr3:uid="{0365826B-1DC9-4904-8CF1-A1C7B2EC0BA0}" name="Ship Qty" dataDxfId="9" dataCellStyle="Calculation">
       <calculatedColumnFormula>SUMIF(Ship_Type[REF], Type[[#This Row],[REF]], Ship_Type[Orders])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{B4A4FBFC-F38A-41E1-97EE-34B2DAD05A6A}" name="Ship Cost" dataDxfId="5" dataCellStyle="Output">
+    <tableColumn id="9" xr3:uid="{B4A4FBFC-F38A-41E1-97EE-34B2DAD05A6A}" name="Ship Cost" dataDxfId="8" dataCellStyle="Output">
       <calculatedColumnFormula>IF(Type[[#This Row],[Ship Code]]="", 0, VLOOKUP(Type[[#This Row],[Ship Code]], Rate[], 3, FALSE)*Type[[#This Row],[Ship Qty]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{ECB96FDD-3FFB-4D2A-B9D7-652E0D8E76B6}" name="Box Code" dataDxfId="4" dataCellStyle="Input"/>
-    <tableColumn id="7" xr3:uid="{61FD82E8-97A0-4340-8DE9-6079A30EA72C}" name="Box Qty" dataDxfId="3" dataCellStyle="Calculation">
+    <tableColumn id="8" xr3:uid="{ECB96FDD-3FFB-4D2A-B9D7-652E0D8E76B6}" name="Box Code" dataDxfId="7" dataCellStyle="Input"/>
+    <tableColumn id="7" xr3:uid="{61FD82E8-97A0-4340-8DE9-6079A30EA72C}" name="Box Qty" dataDxfId="6" dataCellStyle="Calculation">
       <calculatedColumnFormula>SUMIF(Ship_Type[REF], Type[[#This Row],[REF]], Ship_Type[Boxes])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{3E13FEEA-904C-4B08-9F28-1B3E2FCE1F0F}" name="Box Cost" dataDxfId="2" dataCellStyle="Currency">
+    <tableColumn id="5" xr3:uid="{3E13FEEA-904C-4B08-9F28-1B3E2FCE1F0F}" name="Box Cost" dataDxfId="5" dataCellStyle="Currency">
       <calculatedColumnFormula>IF(Type[[#This Row],[Ship Code]]="", 0, VLOOKUP(Type[[#This Row],[Ship Code]], Rate[], 3, FALSE)*Type[[#This Row],[Ship Qty]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{F34217F3-3C8E-4B73-A28F-34E51FFDF408}" name="Cost" dataDxfId="1" dataCellStyle="Output">
+    <tableColumn id="10" xr3:uid="{F34217F3-3C8E-4B73-A28F-34E51FFDF408}" name="Cost" dataDxfId="4" dataCellStyle="Output">
       <calculatedColumnFormula>SUM(Type[[#This Row],[Ship Cost]], Type[[#This Row],[Box Cost]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{8FD79DA1-D3E8-4BF6-A486-3EB465A555C0}" name="Error" dataDxfId="0">
+    <tableColumn id="6" xr3:uid="{8FD79DA1-D3E8-4BF6-A486-3EB465A555C0}" name="Error" dataDxfId="3">
       <calculatedColumnFormula>IF(ISNA(Type[[#This Row],[Box Cost]]), "Error Accessing SAP Rate", "")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1194,9 +1261,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1234,7 +1301,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1340,7 +1407,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1482,7 +1549,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1496,16 +1563,16 @@
   <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N2" sqref="N2"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="32.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1516,7 +1583,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>36</v>
       </c>
@@ -1531,7 +1598,7 @@
         <v/>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>37</v>
       </c>
@@ -1546,7 +1613,7 @@
         <v/>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>38</v>
       </c>
@@ -1561,7 +1628,7 @@
         <v/>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>39</v>
       </c>
@@ -1576,7 +1643,7 @@
         <v/>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>40</v>
       </c>
@@ -1591,35 +1658,35 @@
         <v/>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B7" s="3"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B8" s="3"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B9" s="3"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B10" s="3"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B11" s="3"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B12" s="3"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B13" s="3"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B14" s="3"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B15" s="3"/>
       <c r="G15" s="3"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B16" s="3"/>
     </row>
   </sheetData>
@@ -1646,13 +1713,13 @@
       <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -1666,7 +1733,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>35</v>
       </c>
@@ -1697,28 +1764,28 @@
   <sheetPr codeName="Sheet3">
     <tabColor theme="2" tint="-0.499984740745262"/>
   </sheetPr>
-  <dimension ref="A1:K9"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N2" sqref="N2"/>
+      <selection activeCell="A8" sqref="A8:A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="79.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="79.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="9.7109375" customWidth="1"/>
-    <col min="6" max="6" width="10.5703125" customWidth="1"/>
-    <col min="7" max="7" width="8.85546875" customWidth="1"/>
-    <col min="8" max="8" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="9.6640625" customWidth="1"/>
+    <col min="6" max="6" width="10.5546875" customWidth="1"/>
+    <col min="7" max="7" width="8.88671875" customWidth="1"/>
+    <col min="8" max="8" width="16.5546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="7" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12" customWidth="1"/>
-    <col min="11" max="11" width="26.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="25.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="26.44140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="25.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -1753,15 +1820,15 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>1200122</v>
+        <v>1200112</v>
       </c>
       <c r="B2" t="s">
         <v>41</v>
       </c>
       <c r="C2" s="15">
-        <v>5.95</v>
+        <v>110</v>
       </c>
       <c r="D2" s="12">
         <f>SUMIF(Type[Ship Code], Rate[[#This Row],[SAP Code]], Type[Ship Qty])</f>
@@ -1796,19 +1863,19 @@
         <v/>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>1200112</v>
+        <v>4002222</v>
       </c>
       <c r="B3" t="s">
-        <v>42</v>
+        <v>56</v>
       </c>
       <c r="C3" s="15">
-        <v>110</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="D3" s="12">
         <f>SUMIF(Type[Ship Code], Rate[[#This Row],[SAP Code]], Type[Ship Qty])</f>
-        <v>0</v>
+        <v>5459</v>
       </c>
       <c r="E3" s="12">
         <f>SUMIF(Type[Box Code], Rate[[#This Row],[SAP Code]], Type[Box Qty])</f>
@@ -1828,30 +1895,30 @@
       </c>
       <c r="I3" s="11">
         <f>SUM(Rate[[#This Row],[Orders]:[Commissioned]])</f>
-        <v>0</v>
+        <v>5459</v>
       </c>
       <c r="J3" s="13">
         <f>Rate[[#This Row],[Rate]]*Rate[[#This Row],[Qty]]</f>
-        <v>0</v>
+        <v>27840.899999999998</v>
       </c>
       <c r="K3" t="str">
         <f>IF(ISNA(MATCH(Rate[[#This Row],[SAP Code]], Summary!A:A, 0)), _xlfn.CONCAT("Missing ", Rate[[#This Row],[SAP Code]], " in summary"), "")</f>
         <v/>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>4002222</v>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>57</v>
+        <v>42</v>
       </c>
       <c r="C4" s="15">
-        <v>5.0999999999999996</v>
+        <v>6.2</v>
       </c>
       <c r="D4" s="12">
         <f>SUMIF(Type[Ship Code], Rate[[#This Row],[SAP Code]], Type[Ship Qty])</f>
-        <v>5459</v>
+        <v>0</v>
       </c>
       <c r="E4" s="12">
         <f>SUMIF(Type[Box Code], Rate[[#This Row],[SAP Code]], Type[Box Qty])</f>
@@ -1871,26 +1938,26 @@
       </c>
       <c r="I4" s="11">
         <f>SUM(Rate[[#This Row],[Orders]:[Commissioned]])</f>
-        <v>5459</v>
+        <v>0</v>
       </c>
       <c r="J4" s="13">
         <f>Rate[[#This Row],[Rate]]*Rate[[#This Row],[Qty]]</f>
-        <v>27840.899999999998</v>
+        <v>0</v>
       </c>
       <c r="K4" t="str">
         <f>IF(ISNA(MATCH(Rate[[#This Row],[SAP Code]], Summary!A:A, 0)), _xlfn.CONCAT("Missing ", Rate[[#This Row],[SAP Code]], " in summary"), "")</f>
         <v/>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>5</v>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4002252</v>
       </c>
       <c r="B5" t="s">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="C5" s="15">
-        <v>6.2</v>
+        <v>6.57</v>
       </c>
       <c r="D5" s="12">
         <f>SUMIF(Type[Ship Code], Rate[[#This Row],[SAP Code]], Type[Ship Qty])</f>
@@ -1902,7 +1969,7 @@
       </c>
       <c r="F5" s="12">
         <f>SUMIF(SKU[Ship Code], Rate[[#This Row],[SAP Code]], SKU[Ship Qty])</f>
-        <v>0</v>
+        <v>96</v>
       </c>
       <c r="G5" s="12">
         <f>SUMIF(SKU[Kit Code], Rate[[#This Row],[SAP Code]], SKU[Kit Qty])</f>
@@ -1914,26 +1981,26 @@
       </c>
       <c r="I5" s="11">
         <f>SUM(Rate[[#This Row],[Orders]:[Commissioned]])</f>
-        <v>0</v>
+        <v>96</v>
       </c>
       <c r="J5" s="13">
         <f>Rate[[#This Row],[Rate]]*Rate[[#This Row],[Qty]]</f>
-        <v>0</v>
+        <v>630.72</v>
       </c>
       <c r="K5" t="str">
         <f>IF(ISNA(MATCH(Rate[[#This Row],[SAP Code]], Summary!A:A, 0)), _xlfn.CONCAT("Missing ", Rate[[#This Row],[SAP Code]], " in summary"), "")</f>
         <v/>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>4002252</v>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>43</v>
       </c>
       <c r="B6" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="C6" s="15">
-        <v>6.57</v>
+        <v>1.47</v>
       </c>
       <c r="D6" s="12">
         <f>SUMIF(Type[Ship Code], Rate[[#This Row],[SAP Code]], Type[Ship Qty])</f>
@@ -1945,7 +2012,7 @@
       </c>
       <c r="F6" s="12">
         <f>SUMIF(SKU[Ship Code], Rate[[#This Row],[SAP Code]], SKU[Ship Qty])</f>
-        <v>96</v>
+        <v>0</v>
       </c>
       <c r="G6" s="12">
         <f>SUMIF(SKU[Kit Code], Rate[[#This Row],[SAP Code]], SKU[Kit Qty])</f>
@@ -1957,26 +2024,26 @@
       </c>
       <c r="I6" s="11">
         <f>SUM(Rate[[#This Row],[Orders]:[Commissioned]])</f>
-        <v>96</v>
+        <v>0</v>
       </c>
       <c r="J6" s="13">
         <f>Rate[[#This Row],[Rate]]*Rate[[#This Row],[Qty]]</f>
-        <v>630.72</v>
+        <v>0</v>
       </c>
       <c r="K6" t="str">
         <f>IF(ISNA(MATCH(Rate[[#This Row],[SAP Code]], Summary!A:A, 0)), _xlfn.CONCAT("Missing ", Rate[[#This Row],[SAP Code]], " in summary"), "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>44</v>
-      </c>
-      <c r="B7" t="s">
-        <v>45</v>
+        <v>Missing 400xxxx in summary</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A7" s="33">
+        <v>4002311</v>
+      </c>
+      <c r="B7" s="33" t="s">
+        <v>71</v>
       </c>
       <c r="C7" s="15">
-        <v>1.47</v>
+        <v>5.25</v>
       </c>
       <c r="D7" s="12">
         <f>SUMIF(Type[Ship Code], Rate[[#This Row],[SAP Code]], Type[Ship Qty])</f>
@@ -2008,20 +2075,105 @@
       </c>
       <c r="K7" t="str">
         <f>IF(ISNA(MATCH(Rate[[#This Row],[SAP Code]], Summary!A:A, 0)), _xlfn.CONCAT("Missing ", Rate[[#This Row],[SAP Code]], " in summary"), "")</f>
-        <v>Missing 400xxxx in summary</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="I9" s="16" t="s">
+        <v/>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A8" s="33">
+        <v>4002312</v>
+      </c>
+      <c r="B8" s="33" t="s">
+        <v>72</v>
+      </c>
+      <c r="C8" s="15">
+        <v>5.35</v>
+      </c>
+      <c r="D8" s="12">
+        <f>SUMIF(Type[Ship Code], Rate[[#This Row],[SAP Code]], Type[Ship Qty])</f>
+        <v>0</v>
+      </c>
+      <c r="E8" s="12">
+        <f>SUMIF(Type[Box Code], Rate[[#This Row],[SAP Code]], Type[Box Qty])</f>
+        <v>0</v>
+      </c>
+      <c r="F8" s="12">
+        <f>SUMIF(SKU[Ship Code], Rate[[#This Row],[SAP Code]], SKU[Ship Qty])</f>
+        <v>0</v>
+      </c>
+      <c r="G8" s="12">
+        <f>SUMIF(SKU[Kit Code], Rate[[#This Row],[SAP Code]], SKU[Kit Qty])</f>
+        <v>0</v>
+      </c>
+      <c r="H8" s="12">
+        <f>SUMIF(SKU[Commission Code], Rate[[#This Row],[SAP Code]], SKU[Ship Qty])</f>
+        <v>0</v>
+      </c>
+      <c r="I8" s="11">
+        <f>SUM(Rate[[#This Row],[Orders]:[Commissioned]])</f>
+        <v>0</v>
+      </c>
+      <c r="J8" s="13">
+        <f>Rate[[#This Row],[Rate]]*Rate[[#This Row],[Qty]]</f>
+        <v>0</v>
+      </c>
+      <c r="K8" t="str">
+        <f>IF(ISNA(MATCH(Rate[[#This Row],[SAP Code]], Summary!A:A, 0)), _xlfn.CONCAT("Missing ", Rate[[#This Row],[SAP Code]], " in summary"), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A9" s="34">
+        <v>4002313</v>
+      </c>
+      <c r="B9" s="34" t="s">
+        <v>73</v>
+      </c>
+      <c r="C9" s="35">
+        <v>5.25</v>
+      </c>
+      <c r="D9" s="12">
+        <f>SUMIF(Type[Ship Code], Rate[[#This Row],[SAP Code]], Type[Ship Qty])</f>
+        <v>0</v>
+      </c>
+      <c r="E9" s="12">
+        <f>SUMIF(Type[Box Code], Rate[[#This Row],[SAP Code]], Type[Box Qty])</f>
+        <v>0</v>
+      </c>
+      <c r="F9" s="12">
+        <f>SUMIF(SKU[Ship Code], Rate[[#This Row],[SAP Code]], SKU[Ship Qty])</f>
+        <v>0</v>
+      </c>
+      <c r="G9" s="12">
+        <f>SUMIF(SKU[Kit Code], Rate[[#This Row],[SAP Code]], SKU[Kit Qty])</f>
+        <v>0</v>
+      </c>
+      <c r="H9" s="12">
+        <f>SUMIF(SKU[Commission Code], Rate[[#This Row],[SAP Code]], SKU[Ship Qty])</f>
+        <v>0</v>
+      </c>
+      <c r="I9" s="11">
+        <f>SUM(Rate[[#This Row],[Orders]:[Commissioned]])</f>
+        <v>0</v>
+      </c>
+      <c r="J9" s="13">
+        <f>Rate[[#This Row],[Rate]]*Rate[[#This Row],[Qty]]</f>
+        <v>0</v>
+      </c>
+      <c r="K9" t="str">
+        <f>IF(ISNA(MATCH(Rate[[#This Row],[SAP Code]], Summary!A:A, 0)), _xlfn.CONCAT("Missing ", Rate[[#This Row],[SAP Code]], " in summary"), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="I11" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="J9" s="14">
+      <c r="J11" s="14">
         <f>SUM(Rate[Cost])</f>
         <v>28471.62</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
@@ -2037,26 +2189,26 @@
   <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N2" sqref="N2"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="49.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.85546875" customWidth="1"/>
-    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="11.140625" customWidth="1"/>
-    <col min="10" max="10" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19.28515625" customWidth="1"/>
-    <col min="12" max="12" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="32.7109375" customWidth="1"/>
+    <col min="1" max="1" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="49.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.88671875" customWidth="1"/>
+    <col min="6" max="6" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="11.109375" customWidth="1"/>
+    <col min="10" max="10" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.33203125" customWidth="1"/>
+    <col min="12" max="12" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="32.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2097,12 +2249,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>46</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>47</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="8">
@@ -2139,12 +2291,12 @@
         <v/>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>40</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="8">
@@ -2181,12 +2333,12 @@
         <v/>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>37</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="8">
@@ -2223,12 +2375,12 @@
         <v/>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>38</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="8">
@@ -2265,12 +2417,12 @@
         <v/>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>39</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C6" s="1">
         <v>4002252</v>
@@ -2309,7 +2461,7 @@
         <v/>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>36</v>
       </c>
@@ -2369,20 +2521,20 @@
       <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" customWidth="1"/>
+    <col min="1" max="1" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.109375" customWidth="1"/>
     <col min="4" max="4" width="13" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -2414,12 +2566,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C2" s="31">
         <v>4002222</v>
@@ -2464,22 +2616,22 @@
   <sheetPr codeName="Sheet7">
     <tabColor rgb="FF00B050"/>
   </sheetPr>
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="60.7109375" customWidth="1"/>
+    <col min="1" max="1" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="60.6640625" customWidth="1"/>
     <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="21" t="s">
         <v>3</v>
       </c>
@@ -2496,16 +2648,16 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="32" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B2" s="32"/>
       <c r="C2" s="32"/>
       <c r="D2" s="32"/>
       <c r="E2" s="32"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="27">
         <v>4002222</v>
       </c>
@@ -2526,7 +2678,7 @@
         <v>27351.3</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="28">
         <v>4002252</v>
       </c>
@@ -2547,28 +2699,28 @@
         <v>630.72</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="32" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B6" s="32"/>
       <c r="C6" s="32"/>
       <c r="D6" s="32"/>
       <c r="E6" s="32"/>
     </row>
-    <row r="7" spans="1:5" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="27">
-        <v>1200122</v>
+        <v>4002311</v>
       </c>
       <c r="B7" s="26" t="str">
         <f>VLOOKUP(A7, Rate[[SAP Code]:[Qty]], 2, FALSE)</f>
-        <v>RTS - Processing of RTS Returns, Unpack, Inspection, De-Trash, Scan, Sorting and Report</v>
+        <v>Origin – Processing of RTS Returns – Pristine (Return to Stock)</v>
       </c>
       <c r="C7" s="29">
         <f>VLOOKUP($A7, Rate[[SAP Code]:[Qty]], 3, FALSE)</f>
-        <v>5.95</v>
-      </c>
-      <c r="D7" s="27">
+        <v>5.25</v>
+      </c>
+      <c r="D7" s="36">
         <f>VLOOKUP($A7, Rate[[SAP Code]:[Qty]], 9, FALSE)</f>
         <v>0</v>
       </c>
@@ -2577,73 +2729,115 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E8" s="15"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="32" t="s">
-        <v>55</v>
-      </c>
-      <c r="B9" s="32"/>
-      <c r="C9" s="32"/>
-      <c r="D9" s="32"/>
-      <c r="E9" s="32"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="27" t="s">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="27">
+        <v>4002312</v>
+      </c>
+      <c r="B8" s="26" t="str">
+        <f>VLOOKUP(A8, Rate[[SAP Code]:[Qty]], 2, FALSE)</f>
+        <v xml:space="preserve">Origin – Processing of RTS Returns – Refurbishment Pathway </v>
+      </c>
+      <c r="C8" s="29">
+        <f>VLOOKUP($A8, Rate[[SAP Code]:[Qty]], 3, FALSE)</f>
+        <v>5.35</v>
+      </c>
+      <c r="D8" s="36">
+        <f>VLOOKUP($A8, Rate[[SAP Code]:[Qty]], 9, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="E8" s="29">
+        <f t="shared" ref="E8:E9" si="0">C8*D8</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="27">
+        <v>4002313</v>
+      </c>
+      <c r="B9" s="26" t="str">
+        <f>VLOOKUP(A9, Rate[[SAP Code]:[Qty]], 2, FALSE)</f>
+        <v>Origin – Processing of RTS Returns – BER/Non-Refurbishment</v>
+      </c>
+      <c r="C9" s="29">
+        <f>VLOOKUP($A9, Rate[[SAP Code]:[Qty]], 3, FALSE)</f>
+        <v>5.25</v>
+      </c>
+      <c r="D9" s="36">
+        <f>VLOOKUP($A9, Rate[[SAP Code]:[Qty]], 9, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="E9" s="29">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E10" s="15"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="32" t="s">
+        <v>54</v>
+      </c>
+      <c r="B11" s="32"/>
+      <c r="C11" s="32"/>
+      <c r="D11" s="32"/>
+      <c r="E11" s="32"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="B10" t="str">
-        <f>VLOOKUP(A10, Rate[[SAP Code]:[Qty]], 2, FALSE)</f>
+      <c r="B12" t="str">
+        <f>VLOOKUP(A12, Rate[[SAP Code]:[Qty]], 2, FALSE)</f>
         <v>Standard Pallet Storage</v>
       </c>
-      <c r="C10" s="15">
-        <f>VLOOKUP($A10, Rate[[SAP Code]:[Qty]], 3, FALSE)</f>
+      <c r="C12" s="15">
+        <f>VLOOKUP($A12, Rate[[SAP Code]:[Qty]], 3, FALSE)</f>
         <v>6.2</v>
       </c>
-      <c r="D10" s="23">
-        <f>VLOOKUP($A10, Rate[[SAP Code]:[Qty]], 9, FALSE)</f>
-        <v>0</v>
-      </c>
-      <c r="E10" s="22">
-        <f>C10*D10</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="28">
+      <c r="D12" s="23">
+        <f>VLOOKUP($A12, Rate[[SAP Code]:[Qty]], 9, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="E12" s="22">
+        <f>C12*D12</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="28">
         <v>1200112</v>
       </c>
-      <c r="B11" s="17" t="str">
-        <f>VLOOKUP(A11, Rate[[SAP Code]:[Qty]], 2, FALSE)</f>
+      <c r="B13" s="17" t="str">
+        <f>VLOOKUP(A13, Rate[[SAP Code]:[Qty]], 2, FALSE)</f>
         <v>Labour - Labour Rate Weekday</v>
       </c>
-      <c r="C11" s="20">
-        <f>VLOOKUP($A11, Rate[[SAP Code]:[Qty]], 3, FALSE)</f>
+      <c r="C13" s="20">
+        <f>VLOOKUP($A13, Rate[[SAP Code]:[Qty]], 3, FALSE)</f>
         <v>110</v>
       </c>
-      <c r="D11" s="24">
-        <f>VLOOKUP($A11, Rate[[SAP Code]:[Qty]], 9, FALSE)</f>
-        <v>0</v>
-      </c>
-      <c r="E11" s="20">
-        <f>C11*D11</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="16"/>
-      <c r="C12" s="15"/>
-      <c r="D12" s="15"/>
-      <c r="E12" s="22"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C13" s="19" t="s">
+      <c r="D13" s="24">
+        <f>VLOOKUP($A13, Rate[[SAP Code]:[Qty]], 9, FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="E13" s="20">
+        <f>C13*D13</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" s="16"/>
+      <c r="C14" s="15"/>
+      <c r="D14" s="15"/>
+      <c r="E14" s="22"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C15" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="D13" s="19"/>
-      <c r="E13" s="14">
-        <f>SUM(E3:E11)</f>
+      <c r="D15" s="19"/>
+      <c r="E15" s="14">
+        <f>SUM(E3:E13)</f>
         <v>27982.02</v>
       </c>
     </row>
@@ -2651,7 +2845,7 @@
   <mergeCells count="3">
     <mergeCell ref="A2:E2"/>
     <mergeCell ref="A6:E6"/>
-    <mergeCell ref="A9:E9"/>
+    <mergeCell ref="A11:E11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2669,13 +2863,13 @@
       <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="18" t="s">
         <v>24</v>
       </c>
@@ -2683,7 +2877,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -2692,16 +2886,16 @@
         <v/>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="B3" s="17" t="e">
+      <c r="B3" s="17" t="str">
         <f>_xlfn.IFNA(INDEX(Ship_Type[Error],MATCH(TRUE,INDEX(Ship_Type[Error]&lt;&gt;"",0),0)), "")</f>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v/>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>27</v>
       </c>
@@ -2710,16 +2904,16 @@
         <v/>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="B5" s="17" t="e">
+      <c r="B5" s="17" t="str">
         <f>_xlfn.IFNA(INDEX(Type[Error],MATCH(TRUE,INDEX(Type[Error]&lt;&gt;"",0),0)), "")</f>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+        <v/>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>30</v>
       </c>
@@ -2732,4 +2926,165 @@
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F621C802-4466-412E-A435-E77FBC23A710}">
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" t="s">
+        <v>66</v>
+      </c>
+      <c r="D5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6" t="s">
+        <v>67</v>
+      </c>
+      <c r="D6" t="s">
+        <v>67</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6ED9E796-0C17-4619-9931-4ABD8EE452CB}">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D2" t="s">
+        <v>70</v>
+      </c>
+      <c r="E2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>